<commit_message>
Feito execuções do monkey e calculado os rands
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breno.oliveira\Desktop\IA2019\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>c2ds1-2sp</t>
   </si>
@@ -28,38 +36,190 @@
     <t>average-link</t>
   </si>
   <si>
-    <t>anotar o AR de cada caso</t>
-  </si>
-  <si>
     <t>c2ds3-2g</t>
   </si>
   <si>
     <t>monkey</t>
   </si>
+  <si>
+    <t>0.4554797398007238</t>
+  </si>
+  <si>
+    <t>0.529452639503892</t>
+  </si>
+  <si>
+    <t>0.48884245650686586</t>
+  </si>
+  <si>
+    <t>0.5731801777064264</t>
+  </si>
+  <si>
+    <t>0.6110165713172407</t>
+  </si>
+  <si>
+    <t>0.6336514842661164</t>
+  </si>
+  <si>
+    <t>0.5243234845292539</t>
+  </si>
+  <si>
+    <t>0.6261484128139724</t>
+  </si>
+  <si>
+    <t>0.032887919839679376</t>
+  </si>
+  <si>
+    <t>0.04644337320806546</t>
+  </si>
+  <si>
+    <t>0.0508199430233064</t>
+  </si>
+  <si>
+    <t>0.03474221180330246</t>
+  </si>
+  <si>
+    <t>0.8872515183225375</t>
+  </si>
+  <si>
+    <t>0.4390634040029806</t>
+  </si>
+  <si>
+    <t>0.440449253483619</t>
+  </si>
+  <si>
+    <t>0.3391809285702787</t>
+  </si>
+  <si>
+    <t>0.998001996003992</t>
+  </si>
+  <si>
+    <t>0.996003984015936</t>
+  </si>
+  <si>
+    <t>0.9940099680918327</t>
+  </si>
+  <si>
+    <t>0.03530958733199332</t>
+  </si>
+  <si>
+    <t>0.051768325685199776</t>
+  </si>
+  <si>
+    <t>0.03619551846796416</t>
+  </si>
+  <si>
+    <t>0.030345035932155474</t>
+  </si>
+  <si>
+    <t>0.0003603746454815536</t>
+  </si>
+  <si>
+    <t>0.0003204143703386473</t>
+  </si>
+  <si>
+    <t>0.00025650970764511566</t>
+  </si>
+  <si>
+    <t>0.00022856122260002105</t>
+  </si>
+  <si>
+    <t>0.7359049711544706</t>
+  </si>
+  <si>
+    <t>0.5661971312494792</t>
+  </si>
+  <si>
+    <t>0.413195495681318</t>
+  </si>
+  <si>
+    <t>0.32215296662331094</t>
+  </si>
+  <si>
+    <t>0.5995794532892761</t>
+  </si>
+  <si>
+    <t>0.764390502562894</t>
+  </si>
+  <si>
+    <t>0.8707707222491518</t>
+  </si>
+  <si>
+    <t>0.8344550575452158</t>
+  </si>
+  <si>
+    <t>0.8276670836411557</t>
+  </si>
+  <si>
+    <t>0.8227409963728598</t>
+  </si>
+  <si>
+    <t>0.8221903166270184</t>
+  </si>
+  <si>
+    <t>0.8182816881058694</t>
+  </si>
+  <si>
+    <t>0.46091756738329176</t>
+  </si>
+  <si>
+    <t>0.45121391710425124</t>
+  </si>
+  <si>
+    <t>0.5177170781197129</t>
+  </si>
+  <si>
+    <t>0.5077412482217961</t>
+  </si>
+  <si>
+    <t>0.4724793272074449</t>
+  </si>
+  <si>
+    <t>0.5639546712457681</t>
+  </si>
+  <si>
+    <t>0.5586038059252978</t>
+  </si>
+  <si>
+    <t>0.6929129349731831</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-    </font>
-    <font/>
-    <font>
-      <b/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -67,63 +227,338 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AME1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="4" width="12.71"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1143,7 +1578,7 @@
       <c r="AMD1" s="2"/>
       <c r="AME1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2169,15 +2604,19 @@
       <c r="AMD2" s="2"/>
       <c r="AME2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -3191,13 +3630,19 @@
       <c r="AMD3" s="2"/>
       <c r="AME3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -4211,13 +4656,19 @@
       <c r="AMD4" s="2"/>
       <c r="AME4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -5231,13 +5682,19 @@
       <c r="AMD5" s="2"/>
       <c r="AME5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -6251,7 +6708,7 @@
       <c r="AMD6" s="2"/>
       <c r="AME6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -7269,7 +7726,7 @@
       <c r="AMD7" s="2"/>
       <c r="AME7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -8287,9 +8744,9 @@
       <c r="AMD8" s="2"/>
       <c r="AME8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -9307,7 +9764,7 @@
       <c r="AMD9" s="2"/>
       <c r="AME9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -10333,60 +10790,82 @@
       <c r="AMD10" s="2"/>
       <c r="AME10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4">
-        <v>3.0</v>
+      <c r="B14" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="4">
-        <v>4.0</v>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="4">
-        <v>5.0</v>
+      <c r="D14" s="2" t="s">
+        <v>37</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G15" s="5"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G16" s="5"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
@@ -10401,3003 +10880,3050 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>6.0</v>
+        <v>6</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="5"/>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>7.0</v>
+        <v>7</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="G21" s="5"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>8.0</v>
+        <v>8</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="5"/>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="G23" s="5"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>10.0</v>
+        <v>10</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="5"/>
+      <c r="B24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="G24" s="5"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>11.0</v>
+        <v>11</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>12.0</v>
+        <v>12</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="5"/>
+      <c r="B26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="G26" s="5"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G27" s="5"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G28" s="5"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G29" s="5"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G30" s="5"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G31" s="5"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G32" s="5"/>
     </row>
-    <row r="33">
+    <row r="33" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G33" s="5"/>
     </row>
-    <row r="34">
+    <row r="34" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G34" s="5"/>
     </row>
-    <row r="35">
+    <row r="35" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G35" s="5"/>
     </row>
-    <row r="36">
+    <row r="36" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G36" s="5"/>
     </row>
-    <row r="37">
+    <row r="37" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G37" s="5"/>
     </row>
-    <row r="38">
+    <row r="38" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G38" s="5"/>
     </row>
-    <row r="39">
+    <row r="39" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G39" s="5"/>
     </row>
-    <row r="40">
+    <row r="40" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G40" s="5"/>
     </row>
-    <row r="41">
+    <row r="41" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G41" s="5"/>
     </row>
-    <row r="42">
+    <row r="42" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G42" s="5"/>
     </row>
-    <row r="43">
+    <row r="43" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G43" s="5"/>
     </row>
-    <row r="44">
+    <row r="44" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G44" s="5"/>
     </row>
-    <row r="45">
+    <row r="45" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G45" s="5"/>
     </row>
-    <row r="46">
+    <row r="46" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G46" s="5"/>
     </row>
-    <row r="47">
+    <row r="47" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G47" s="5"/>
     </row>
-    <row r="48">
+    <row r="48" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G48" s="5"/>
     </row>
-    <row r="49">
+    <row r="49" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G49" s="5"/>
     </row>
-    <row r="50">
+    <row r="50" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G50" s="5"/>
     </row>
-    <row r="51">
+    <row r="51" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G51" s="5"/>
     </row>
-    <row r="52">
+    <row r="52" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G52" s="5"/>
     </row>
-    <row r="53">
+    <row r="53" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G53" s="5"/>
     </row>
-    <row r="54">
+    <row r="54" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G54" s="5"/>
     </row>
-    <row r="55">
+    <row r="55" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G55" s="5"/>
     </row>
-    <row r="56">
+    <row r="56" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G56" s="5"/>
     </row>
-    <row r="57">
+    <row r="57" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G57" s="5"/>
     </row>
-    <row r="58">
+    <row r="58" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G58" s="5"/>
     </row>
-    <row r="59">
+    <row r="59" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G59" s="5"/>
     </row>
-    <row r="60">
+    <row r="60" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G60" s="5"/>
     </row>
-    <row r="61">
+    <row r="61" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G61" s="5"/>
     </row>
-    <row r="62">
+    <row r="62" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G62" s="5"/>
     </row>
-    <row r="63">
+    <row r="63" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G63" s="5"/>
     </row>
-    <row r="64">
+    <row r="64" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G64" s="5"/>
     </row>
-    <row r="65">
+    <row r="65" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G65" s="5"/>
     </row>
-    <row r="66">
+    <row r="66" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G66" s="5"/>
     </row>
-    <row r="67">
+    <row r="67" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G67" s="5"/>
     </row>
-    <row r="68">
+    <row r="68" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G68" s="5"/>
     </row>
-    <row r="69">
+    <row r="69" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G69" s="5"/>
     </row>
-    <row r="70">
+    <row r="70" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G70" s="5"/>
     </row>
-    <row r="71">
+    <row r="71" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G71" s="5"/>
     </row>
-    <row r="72">
+    <row r="72" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G72" s="5"/>
     </row>
-    <row r="73">
+    <row r="73" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G73" s="5"/>
     </row>
-    <row r="74">
+    <row r="74" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G74" s="5"/>
     </row>
-    <row r="75">
+    <row r="75" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G75" s="5"/>
     </row>
-    <row r="76">
+    <row r="76" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G76" s="5"/>
     </row>
-    <row r="77">
+    <row r="77" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G77" s="5"/>
     </row>
-    <row r="78">
+    <row r="78" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G78" s="5"/>
     </row>
-    <row r="79">
+    <row r="79" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G79" s="5"/>
     </row>
-    <row r="80">
+    <row r="80" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G80" s="5"/>
     </row>
-    <row r="81">
+    <row r="81" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G81" s="5"/>
     </row>
-    <row r="82">
+    <row r="82" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G82" s="5"/>
     </row>
-    <row r="83">
+    <row r="83" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G83" s="5"/>
     </row>
-    <row r="84">
+    <row r="84" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G84" s="5"/>
     </row>
-    <row r="85">
+    <row r="85" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G85" s="5"/>
     </row>
-    <row r="86">
+    <row r="86" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G86" s="5"/>
     </row>
-    <row r="87">
+    <row r="87" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G87" s="5"/>
     </row>
-    <row r="88">
+    <row r="88" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G88" s="5"/>
     </row>
-    <row r="89">
+    <row r="89" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G89" s="5"/>
     </row>
-    <row r="90">
+    <row r="90" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G90" s="5"/>
     </row>
-    <row r="91">
+    <row r="91" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G91" s="5"/>
     </row>
-    <row r="92">
+    <row r="92" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G92" s="5"/>
     </row>
-    <row r="93">
+    <row r="93" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G93" s="5"/>
     </row>
-    <row r="94">
+    <row r="94" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G94" s="5"/>
     </row>
-    <row r="95">
+    <row r="95" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G95" s="5"/>
     </row>
-    <row r="96">
+    <row r="96" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G96" s="5"/>
     </row>
-    <row r="97">
+    <row r="97" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G97" s="5"/>
     </row>
-    <row r="98">
+    <row r="98" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G98" s="5"/>
     </row>
-    <row r="99">
+    <row r="99" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G99" s="5"/>
     </row>
-    <row r="100">
+    <row r="100" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G100" s="5"/>
     </row>
-    <row r="101">
+    <row r="101" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G101" s="5"/>
     </row>
-    <row r="102">
+    <row r="102" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G102" s="5"/>
     </row>
-    <row r="103">
+    <row r="103" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G103" s="5"/>
     </row>
-    <row r="104">
+    <row r="104" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G104" s="5"/>
     </row>
-    <row r="105">
+    <row r="105" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G105" s="5"/>
     </row>
-    <row r="106">
+    <row r="106" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G106" s="5"/>
     </row>
-    <row r="107">
+    <row r="107" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G107" s="5"/>
     </row>
-    <row r="108">
+    <row r="108" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G108" s="5"/>
     </row>
-    <row r="109">
+    <row r="109" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G109" s="5"/>
     </row>
-    <row r="110">
+    <row r="110" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G110" s="5"/>
     </row>
-    <row r="111">
+    <row r="111" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G111" s="5"/>
     </row>
-    <row r="112">
+    <row r="112" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G112" s="5"/>
     </row>
-    <row r="113">
+    <row r="113" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G113" s="5"/>
     </row>
-    <row r="114">
+    <row r="114" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G114" s="5"/>
     </row>
-    <row r="115">
+    <row r="115" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G115" s="5"/>
     </row>
-    <row r="116">
+    <row r="116" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G116" s="5"/>
     </row>
-    <row r="117">
+    <row r="117" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G117" s="5"/>
     </row>
-    <row r="118">
+    <row r="118" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G118" s="5"/>
     </row>
-    <row r="119">
+    <row r="119" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G119" s="5"/>
     </row>
-    <row r="120">
+    <row r="120" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G120" s="5"/>
     </row>
-    <row r="121">
+    <row r="121" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G121" s="5"/>
     </row>
-    <row r="122">
+    <row r="122" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G122" s="5"/>
     </row>
-    <row r="123">
+    <row r="123" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G123" s="5"/>
     </row>
-    <row r="124">
+    <row r="124" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G124" s="5"/>
     </row>
-    <row r="125">
+    <row r="125" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G125" s="5"/>
     </row>
-    <row r="126">
+    <row r="126" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G126" s="5"/>
     </row>
-    <row r="127">
+    <row r="127" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G127" s="5"/>
     </row>
-    <row r="128">
+    <row r="128" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G128" s="5"/>
     </row>
-    <row r="129">
+    <row r="129" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G129" s="5"/>
     </row>
-    <row r="130">
+    <row r="130" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G130" s="5"/>
     </row>
-    <row r="131">
+    <row r="131" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G131" s="5"/>
     </row>
-    <row r="132">
+    <row r="132" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G132" s="5"/>
     </row>
-    <row r="133">
+    <row r="133" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G133" s="5"/>
     </row>
-    <row r="134">
+    <row r="134" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G134" s="5"/>
     </row>
-    <row r="135">
+    <row r="135" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G135" s="5"/>
     </row>
-    <row r="136">
+    <row r="136" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G136" s="5"/>
     </row>
-    <row r="137">
+    <row r="137" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G137" s="5"/>
     </row>
-    <row r="138">
+    <row r="138" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G138" s="5"/>
     </row>
-    <row r="139">
+    <row r="139" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G139" s="5"/>
     </row>
-    <row r="140">
+    <row r="140" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G140" s="5"/>
     </row>
-    <row r="141">
+    <row r="141" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G141" s="5"/>
     </row>
-    <row r="142">
+    <row r="142" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G142" s="5"/>
     </row>
-    <row r="143">
+    <row r="143" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G143" s="5"/>
     </row>
-    <row r="144">
+    <row r="144" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G144" s="5"/>
     </row>
-    <row r="145">
+    <row r="145" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G145" s="5"/>
     </row>
-    <row r="146">
+    <row r="146" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G146" s="5"/>
     </row>
-    <row r="147">
+    <row r="147" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G147" s="5"/>
     </row>
-    <row r="148">
+    <row r="148" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G148" s="5"/>
     </row>
-    <row r="149">
+    <row r="149" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G149" s="5"/>
     </row>
-    <row r="150">
+    <row r="150" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G150" s="5"/>
     </row>
-    <row r="151">
+    <row r="151" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G151" s="5"/>
     </row>
-    <row r="152">
+    <row r="152" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G152" s="5"/>
     </row>
-    <row r="153">
+    <row r="153" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G153" s="5"/>
     </row>
-    <row r="154">
+    <row r="154" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G154" s="5"/>
     </row>
-    <row r="155">
+    <row r="155" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G155" s="5"/>
     </row>
-    <row r="156">
+    <row r="156" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G156" s="5"/>
     </row>
-    <row r="157">
+    <row r="157" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G157" s="5"/>
     </row>
-    <row r="158">
+    <row r="158" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G158" s="5"/>
     </row>
-    <row r="159">
+    <row r="159" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G159" s="5"/>
     </row>
-    <row r="160">
+    <row r="160" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G160" s="5"/>
     </row>
-    <row r="161">
+    <row r="161" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G161" s="5"/>
     </row>
-    <row r="162">
+    <row r="162" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G162" s="5"/>
     </row>
-    <row r="163">
+    <row r="163" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G163" s="5"/>
     </row>
-    <row r="164">
+    <row r="164" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G164" s="5"/>
     </row>
-    <row r="165">
+    <row r="165" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G165" s="5"/>
     </row>
-    <row r="166">
+    <row r="166" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G166" s="5"/>
     </row>
-    <row r="167">
+    <row r="167" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G167" s="5"/>
     </row>
-    <row r="168">
+    <row r="168" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G168" s="5"/>
     </row>
-    <row r="169">
+    <row r="169" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G169" s="5"/>
     </row>
-    <row r="170">
+    <row r="170" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G170" s="5"/>
     </row>
-    <row r="171">
+    <row r="171" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G171" s="5"/>
     </row>
-    <row r="172">
+    <row r="172" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G172" s="5"/>
     </row>
-    <row r="173">
+    <row r="173" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G173" s="5"/>
     </row>
-    <row r="174">
+    <row r="174" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G174" s="5"/>
     </row>
-    <row r="175">
+    <row r="175" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G175" s="5"/>
     </row>
-    <row r="176">
+    <row r="176" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G176" s="5"/>
     </row>
-    <row r="177">
+    <row r="177" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G177" s="5"/>
     </row>
-    <row r="178">
+    <row r="178" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G178" s="5"/>
     </row>
-    <row r="179">
+    <row r="179" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G179" s="5"/>
     </row>
-    <row r="180">
+    <row r="180" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G180" s="5"/>
     </row>
-    <row r="181">
+    <row r="181" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G181" s="5"/>
     </row>
-    <row r="182">
+    <row r="182" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G182" s="5"/>
     </row>
-    <row r="183">
+    <row r="183" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G183" s="5"/>
     </row>
-    <row r="184">
+    <row r="184" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G184" s="5"/>
     </row>
-    <row r="185">
+    <row r="185" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G185" s="5"/>
     </row>
-    <row r="186">
+    <row r="186" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G186" s="5"/>
     </row>
-    <row r="187">
+    <row r="187" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G187" s="5"/>
     </row>
-    <row r="188">
+    <row r="188" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G188" s="5"/>
     </row>
-    <row r="189">
+    <row r="189" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G189" s="5"/>
     </row>
-    <row r="190">
+    <row r="190" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G190" s="5"/>
     </row>
-    <row r="191">
+    <row r="191" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G191" s="5"/>
     </row>
-    <row r="192">
+    <row r="192" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G192" s="5"/>
     </row>
-    <row r="193">
+    <row r="193" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G193" s="5"/>
     </row>
-    <row r="194">
+    <row r="194" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G194" s="5"/>
     </row>
-    <row r="195">
+    <row r="195" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G195" s="5"/>
     </row>
-    <row r="196">
+    <row r="196" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G196" s="5"/>
     </row>
-    <row r="197">
+    <row r="197" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G197" s="5"/>
     </row>
-    <row r="198">
+    <row r="198" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G198" s="5"/>
     </row>
-    <row r="199">
+    <row r="199" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G199" s="5"/>
     </row>
-    <row r="200">
+    <row r="200" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G200" s="5"/>
     </row>
-    <row r="201">
+    <row r="201" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G201" s="5"/>
     </row>
-    <row r="202">
+    <row r="202" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G202" s="5"/>
     </row>
-    <row r="203">
+    <row r="203" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G203" s="5"/>
     </row>
-    <row r="204">
+    <row r="204" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G204" s="5"/>
     </row>
-    <row r="205">
+    <row r="205" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G205" s="5"/>
     </row>
-    <row r="206">
+    <row r="206" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G206" s="5"/>
     </row>
-    <row r="207">
+    <row r="207" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G207" s="5"/>
     </row>
-    <row r="208">
+    <row r="208" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G208" s="5"/>
     </row>
-    <row r="209">
+    <row r="209" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G209" s="5"/>
     </row>
-    <row r="210">
+    <row r="210" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G210" s="5"/>
     </row>
-    <row r="211">
+    <row r="211" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G211" s="5"/>
     </row>
-    <row r="212">
+    <row r="212" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G212" s="5"/>
     </row>
-    <row r="213">
+    <row r="213" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G213" s="5"/>
     </row>
-    <row r="214">
+    <row r="214" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G214" s="5"/>
     </row>
-    <row r="215">
+    <row r="215" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G215" s="5"/>
     </row>
-    <row r="216">
+    <row r="216" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G216" s="5"/>
     </row>
-    <row r="217">
+    <row r="217" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G217" s="5"/>
     </row>
-    <row r="218">
+    <row r="218" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G218" s="5"/>
     </row>
-    <row r="219">
+    <row r="219" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G219" s="5"/>
     </row>
-    <row r="220">
+    <row r="220" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G220" s="5"/>
     </row>
-    <row r="221">
+    <row r="221" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G221" s="5"/>
     </row>
-    <row r="222">
+    <row r="222" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G222" s="5"/>
     </row>
-    <row r="223">
+    <row r="223" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G223" s="5"/>
     </row>
-    <row r="224">
+    <row r="224" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G224" s="5"/>
     </row>
-    <row r="225">
+    <row r="225" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G225" s="5"/>
     </row>
-    <row r="226">
+    <row r="226" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G226" s="5"/>
     </row>
-    <row r="227">
+    <row r="227" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G227" s="5"/>
     </row>
-    <row r="228">
+    <row r="228" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G228" s="5"/>
     </row>
-    <row r="229">
+    <row r="229" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G229" s="5"/>
     </row>
-    <row r="230">
+    <row r="230" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G230" s="5"/>
     </row>
-    <row r="231">
+    <row r="231" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G231" s="5"/>
     </row>
-    <row r="232">
+    <row r="232" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G232" s="5"/>
     </row>
-    <row r="233">
+    <row r="233" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G233" s="5"/>
     </row>
-    <row r="234">
+    <row r="234" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G234" s="5"/>
     </row>
-    <row r="235">
+    <row r="235" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G235" s="5"/>
     </row>
-    <row r="236">
+    <row r="236" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G236" s="5"/>
     </row>
-    <row r="237">
+    <row r="237" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G237" s="5"/>
     </row>
-    <row r="238">
+    <row r="238" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G238" s="5"/>
     </row>
-    <row r="239">
+    <row r="239" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G239" s="5"/>
     </row>
-    <row r="240">
+    <row r="240" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G240" s="5"/>
     </row>
-    <row r="241">
+    <row r="241" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G241" s="5"/>
     </row>
-    <row r="242">
+    <row r="242" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G242" s="5"/>
     </row>
-    <row r="243">
+    <row r="243" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G243" s="5"/>
     </row>
-    <row r="244">
+    <row r="244" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G244" s="5"/>
     </row>
-    <row r="245">
+    <row r="245" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G245" s="5"/>
     </row>
-    <row r="246">
+    <row r="246" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G246" s="5"/>
     </row>
-    <row r="247">
+    <row r="247" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G247" s="5"/>
     </row>
-    <row r="248">
+    <row r="248" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G248" s="5"/>
     </row>
-    <row r="249">
+    <row r="249" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G249" s="5"/>
     </row>
-    <row r="250">
+    <row r="250" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G250" s="5"/>
     </row>
-    <row r="251">
+    <row r="251" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G251" s="5"/>
     </row>
-    <row r="252">
+    <row r="252" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G252" s="5"/>
     </row>
-    <row r="253">
+    <row r="253" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G253" s="5"/>
     </row>
-    <row r="254">
+    <row r="254" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G254" s="5"/>
     </row>
-    <row r="255">
+    <row r="255" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G255" s="5"/>
     </row>
-    <row r="256">
+    <row r="256" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G256" s="5"/>
     </row>
-    <row r="257">
+    <row r="257" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G257" s="5"/>
     </row>
-    <row r="258">
+    <row r="258" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G258" s="5"/>
     </row>
-    <row r="259">
+    <row r="259" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G259" s="5"/>
     </row>
-    <row r="260">
+    <row r="260" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G260" s="5"/>
     </row>
-    <row r="261">
+    <row r="261" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G261" s="5"/>
     </row>
-    <row r="262">
+    <row r="262" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G262" s="5"/>
     </row>
-    <row r="263">
+    <row r="263" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G263" s="5"/>
     </row>
-    <row r="264">
+    <row r="264" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G264" s="5"/>
     </row>
-    <row r="265">
+    <row r="265" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G265" s="5"/>
     </row>
-    <row r="266">
+    <row r="266" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G266" s="5"/>
     </row>
-    <row r="267">
+    <row r="267" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G267" s="5"/>
     </row>
-    <row r="268">
+    <row r="268" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G268" s="5"/>
     </row>
-    <row r="269">
+    <row r="269" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G269" s="5"/>
     </row>
-    <row r="270">
+    <row r="270" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G270" s="5"/>
     </row>
-    <row r="271">
+    <row r="271" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G271" s="5"/>
     </row>
-    <row r="272">
+    <row r="272" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G272" s="5"/>
     </row>
-    <row r="273">
+    <row r="273" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G273" s="5"/>
     </row>
-    <row r="274">
+    <row r="274" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G274" s="5"/>
     </row>
-    <row r="275">
+    <row r="275" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G275" s="5"/>
     </row>
-    <row r="276">
+    <row r="276" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G276" s="5"/>
     </row>
-    <row r="277">
+    <row r="277" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G277" s="5"/>
     </row>
-    <row r="278">
+    <row r="278" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G278" s="5"/>
     </row>
-    <row r="279">
+    <row r="279" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G279" s="5"/>
     </row>
-    <row r="280">
+    <row r="280" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G280" s="5"/>
     </row>
-    <row r="281">
+    <row r="281" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G281" s="5"/>
     </row>
-    <row r="282">
+    <row r="282" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G282" s="5"/>
     </row>
-    <row r="283">
+    <row r="283" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G283" s="5"/>
     </row>
-    <row r="284">
+    <row r="284" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G284" s="5"/>
     </row>
-    <row r="285">
+    <row r="285" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G285" s="5"/>
     </row>
-    <row r="286">
+    <row r="286" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G286" s="5"/>
     </row>
-    <row r="287">
+    <row r="287" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G287" s="5"/>
     </row>
-    <row r="288">
+    <row r="288" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G288" s="5"/>
     </row>
-    <row r="289">
+    <row r="289" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G289" s="5"/>
     </row>
-    <row r="290">
+    <row r="290" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G290" s="5"/>
     </row>
-    <row r="291">
+    <row r="291" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G291" s="5"/>
     </row>
-    <row r="292">
+    <row r="292" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G292" s="5"/>
     </row>
-    <row r="293">
+    <row r="293" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G293" s="5"/>
     </row>
-    <row r="294">
+    <row r="294" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G294" s="5"/>
     </row>
-    <row r="295">
+    <row r="295" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G295" s="5"/>
     </row>
-    <row r="296">
+    <row r="296" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G296" s="5"/>
     </row>
-    <row r="297">
+    <row r="297" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G297" s="5"/>
     </row>
-    <row r="298">
+    <row r="298" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G298" s="5"/>
     </row>
-    <row r="299">
+    <row r="299" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G299" s="5"/>
     </row>
-    <row r="300">
+    <row r="300" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G300" s="5"/>
     </row>
-    <row r="301">
+    <row r="301" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G301" s="5"/>
     </row>
-    <row r="302">
+    <row r="302" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G302" s="5"/>
     </row>
-    <row r="303">
+    <row r="303" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G303" s="5"/>
     </row>
-    <row r="304">
+    <row r="304" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G304" s="5"/>
     </row>
-    <row r="305">
+    <row r="305" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G305" s="5"/>
     </row>
-    <row r="306">
+    <row r="306" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G306" s="5"/>
     </row>
-    <row r="307">
+    <row r="307" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G307" s="5"/>
     </row>
-    <row r="308">
+    <row r="308" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G308" s="5"/>
     </row>
-    <row r="309">
+    <row r="309" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G309" s="5"/>
     </row>
-    <row r="310">
+    <row r="310" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G310" s="5"/>
     </row>
-    <row r="311">
+    <row r="311" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G311" s="5"/>
     </row>
-    <row r="312">
+    <row r="312" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G312" s="5"/>
     </row>
-    <row r="313">
+    <row r="313" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G313" s="5"/>
     </row>
-    <row r="314">
+    <row r="314" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G314" s="5"/>
     </row>
-    <row r="315">
+    <row r="315" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G315" s="5"/>
     </row>
-    <row r="316">
+    <row r="316" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G316" s="5"/>
     </row>
-    <row r="317">
+    <row r="317" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G317" s="5"/>
     </row>
-    <row r="318">
+    <row r="318" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G318" s="5"/>
     </row>
-    <row r="319">
+    <row r="319" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G319" s="5"/>
     </row>
-    <row r="320">
+    <row r="320" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G320" s="5"/>
     </row>
-    <row r="321">
+    <row r="321" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G321" s="5"/>
     </row>
-    <row r="322">
+    <row r="322" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G322" s="5"/>
     </row>
-    <row r="323">
+    <row r="323" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G323" s="5"/>
     </row>
-    <row r="324">
+    <row r="324" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G324" s="5"/>
     </row>
-    <row r="325">
+    <row r="325" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G325" s="5"/>
     </row>
-    <row r="326">
+    <row r="326" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G326" s="5"/>
     </row>
-    <row r="327">
+    <row r="327" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G327" s="5"/>
     </row>
-    <row r="328">
+    <row r="328" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G328" s="5"/>
     </row>
-    <row r="329">
+    <row r="329" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G329" s="5"/>
     </row>
-    <row r="330">
+    <row r="330" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G330" s="5"/>
     </row>
-    <row r="331">
+    <row r="331" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G331" s="5"/>
     </row>
-    <row r="332">
+    <row r="332" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G332" s="5"/>
     </row>
-    <row r="333">
+    <row r="333" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G333" s="5"/>
     </row>
-    <row r="334">
+    <row r="334" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G334" s="5"/>
     </row>
-    <row r="335">
+    <row r="335" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G335" s="5"/>
     </row>
-    <row r="336">
+    <row r="336" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G336" s="5"/>
     </row>
-    <row r="337">
+    <row r="337" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G337" s="5"/>
     </row>
-    <row r="338">
+    <row r="338" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G338" s="5"/>
     </row>
-    <row r="339">
+    <row r="339" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G339" s="5"/>
     </row>
-    <row r="340">
+    <row r="340" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G340" s="5"/>
     </row>
-    <row r="341">
+    <row r="341" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G341" s="5"/>
     </row>
-    <row r="342">
+    <row r="342" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G342" s="5"/>
     </row>
-    <row r="343">
+    <row r="343" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G343" s="5"/>
     </row>
-    <row r="344">
+    <row r="344" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G344" s="5"/>
     </row>
-    <row r="345">
+    <row r="345" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G345" s="5"/>
     </row>
-    <row r="346">
+    <row r="346" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G346" s="5"/>
     </row>
-    <row r="347">
+    <row r="347" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G347" s="5"/>
     </row>
-    <row r="348">
+    <row r="348" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G348" s="5"/>
     </row>
-    <row r="349">
+    <row r="349" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G349" s="5"/>
     </row>
-    <row r="350">
+    <row r="350" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G350" s="5"/>
     </row>
-    <row r="351">
+    <row r="351" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G351" s="5"/>
     </row>
-    <row r="352">
+    <row r="352" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G352" s="5"/>
     </row>
-    <row r="353">
+    <row r="353" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G353" s="5"/>
     </row>
-    <row r="354">
+    <row r="354" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G354" s="5"/>
     </row>
-    <row r="355">
+    <row r="355" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G355" s="5"/>
     </row>
-    <row r="356">
+    <row r="356" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G356" s="5"/>
     </row>
-    <row r="357">
+    <row r="357" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G357" s="5"/>
     </row>
-    <row r="358">
+    <row r="358" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G358" s="5"/>
     </row>
-    <row r="359">
+    <row r="359" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G359" s="5"/>
     </row>
-    <row r="360">
+    <row r="360" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G360" s="5"/>
     </row>
-    <row r="361">
+    <row r="361" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G361" s="5"/>
     </row>
-    <row r="362">
+    <row r="362" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G362" s="5"/>
     </row>
-    <row r="363">
+    <row r="363" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G363" s="5"/>
     </row>
-    <row r="364">
+    <row r="364" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G364" s="5"/>
     </row>
-    <row r="365">
+    <row r="365" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G365" s="5"/>
     </row>
-    <row r="366">
+    <row r="366" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G366" s="5"/>
     </row>
-    <row r="367">
+    <row r="367" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G367" s="5"/>
     </row>
-    <row r="368">
+    <row r="368" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G368" s="5"/>
     </row>
-    <row r="369">
+    <row r="369" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G369" s="5"/>
     </row>
-    <row r="370">
+    <row r="370" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G370" s="5"/>
     </row>
-    <row r="371">
+    <row r="371" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G371" s="5"/>
     </row>
-    <row r="372">
+    <row r="372" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G372" s="5"/>
     </row>
-    <row r="373">
+    <row r="373" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G373" s="5"/>
     </row>
-    <row r="374">
+    <row r="374" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G374" s="5"/>
     </row>
-    <row r="375">
+    <row r="375" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G375" s="5"/>
     </row>
-    <row r="376">
+    <row r="376" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G376" s="5"/>
     </row>
-    <row r="377">
+    <row r="377" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G377" s="5"/>
     </row>
-    <row r="378">
+    <row r="378" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G378" s="5"/>
     </row>
-    <row r="379">
+    <row r="379" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G379" s="5"/>
     </row>
-    <row r="380">
+    <row r="380" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G380" s="5"/>
     </row>
-    <row r="381">
+    <row r="381" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G381" s="5"/>
     </row>
-    <row r="382">
+    <row r="382" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G382" s="5"/>
     </row>
-    <row r="383">
+    <row r="383" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G383" s="5"/>
     </row>
-    <row r="384">
+    <row r="384" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G384" s="5"/>
     </row>
-    <row r="385">
+    <row r="385" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G385" s="5"/>
     </row>
-    <row r="386">
+    <row r="386" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G386" s="5"/>
     </row>
-    <row r="387">
+    <row r="387" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G387" s="5"/>
     </row>
-    <row r="388">
+    <row r="388" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G388" s="5"/>
     </row>
-    <row r="389">
+    <row r="389" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G389" s="5"/>
     </row>
-    <row r="390">
+    <row r="390" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G390" s="5"/>
     </row>
-    <row r="391">
+    <row r="391" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G391" s="5"/>
     </row>
-    <row r="392">
+    <row r="392" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G392" s="5"/>
     </row>
-    <row r="393">
+    <row r="393" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G393" s="5"/>
     </row>
-    <row r="394">
+    <row r="394" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G394" s="5"/>
     </row>
-    <row r="395">
+    <row r="395" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G395" s="5"/>
     </row>
-    <row r="396">
+    <row r="396" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G396" s="5"/>
     </row>
-    <row r="397">
+    <row r="397" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G397" s="5"/>
     </row>
-    <row r="398">
+    <row r="398" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G398" s="5"/>
     </row>
-    <row r="399">
+    <row r="399" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G399" s="5"/>
     </row>
-    <row r="400">
+    <row r="400" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G400" s="5"/>
     </row>
-    <row r="401">
+    <row r="401" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G401" s="5"/>
     </row>
-    <row r="402">
+    <row r="402" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G402" s="5"/>
     </row>
-    <row r="403">
+    <row r="403" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G403" s="5"/>
     </row>
-    <row r="404">
+    <row r="404" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G404" s="5"/>
     </row>
-    <row r="405">
+    <row r="405" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G405" s="5"/>
     </row>
-    <row r="406">
+    <row r="406" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G406" s="5"/>
     </row>
-    <row r="407">
+    <row r="407" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G407" s="5"/>
     </row>
-    <row r="408">
+    <row r="408" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G408" s="5"/>
     </row>
-    <row r="409">
+    <row r="409" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G409" s="5"/>
     </row>
-    <row r="410">
+    <row r="410" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G410" s="5"/>
     </row>
-    <row r="411">
+    <row r="411" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G411" s="5"/>
     </row>
-    <row r="412">
+    <row r="412" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G412" s="5"/>
     </row>
-    <row r="413">
+    <row r="413" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G413" s="5"/>
     </row>
-    <row r="414">
+    <row r="414" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G414" s="5"/>
     </row>
-    <row r="415">
+    <row r="415" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G415" s="5"/>
     </row>
-    <row r="416">
+    <row r="416" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G416" s="5"/>
     </row>
-    <row r="417">
+    <row r="417" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G417" s="5"/>
     </row>
-    <row r="418">
+    <row r="418" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G418" s="5"/>
     </row>
-    <row r="419">
+    <row r="419" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G419" s="5"/>
     </row>
-    <row r="420">
+    <row r="420" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G420" s="5"/>
     </row>
-    <row r="421">
+    <row r="421" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G421" s="5"/>
     </row>
-    <row r="422">
+    <row r="422" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G422" s="5"/>
     </row>
-    <row r="423">
+    <row r="423" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G423" s="5"/>
     </row>
-    <row r="424">
+    <row r="424" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G424" s="5"/>
     </row>
-    <row r="425">
+    <row r="425" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G425" s="5"/>
     </row>
-    <row r="426">
+    <row r="426" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G426" s="5"/>
     </row>
-    <row r="427">
+    <row r="427" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G427" s="5"/>
     </row>
-    <row r="428">
+    <row r="428" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G428" s="5"/>
     </row>
-    <row r="429">
+    <row r="429" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G429" s="5"/>
     </row>
-    <row r="430">
+    <row r="430" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G430" s="5"/>
     </row>
-    <row r="431">
+    <row r="431" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G431" s="5"/>
     </row>
-    <row r="432">
+    <row r="432" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G432" s="5"/>
     </row>
-    <row r="433">
+    <row r="433" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G433" s="5"/>
     </row>
-    <row r="434">
+    <row r="434" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G434" s="5"/>
     </row>
-    <row r="435">
+    <row r="435" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G435" s="5"/>
     </row>
-    <row r="436">
+    <row r="436" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G436" s="5"/>
     </row>
-    <row r="437">
+    <row r="437" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G437" s="5"/>
     </row>
-    <row r="438">
+    <row r="438" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G438" s="5"/>
     </row>
-    <row r="439">
+    <row r="439" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G439" s="5"/>
     </row>
-    <row r="440">
+    <row r="440" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G440" s="5"/>
     </row>
-    <row r="441">
+    <row r="441" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G441" s="5"/>
     </row>
-    <row r="442">
+    <row r="442" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G442" s="5"/>
     </row>
-    <row r="443">
+    <row r="443" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G443" s="5"/>
     </row>
-    <row r="444">
+    <row r="444" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G444" s="5"/>
     </row>
-    <row r="445">
+    <row r="445" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G445" s="5"/>
     </row>
-    <row r="446">
+    <row r="446" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G446" s="5"/>
     </row>
-    <row r="447">
+    <row r="447" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G447" s="5"/>
     </row>
-    <row r="448">
+    <row r="448" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G448" s="5"/>
     </row>
-    <row r="449">
+    <row r="449" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G449" s="5"/>
     </row>
-    <row r="450">
+    <row r="450" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G450" s="5"/>
     </row>
-    <row r="451">
+    <row r="451" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G451" s="5"/>
     </row>
-    <row r="452">
+    <row r="452" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G452" s="5"/>
     </row>
-    <row r="453">
+    <row r="453" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G453" s="5"/>
     </row>
-    <row r="454">
+    <row r="454" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G454" s="5"/>
     </row>
-    <row r="455">
+    <row r="455" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G455" s="5"/>
     </row>
-    <row r="456">
+    <row r="456" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G456" s="5"/>
     </row>
-    <row r="457">
+    <row r="457" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G457" s="5"/>
     </row>
-    <row r="458">
+    <row r="458" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G458" s="5"/>
     </row>
-    <row r="459">
+    <row r="459" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G459" s="5"/>
     </row>
-    <row r="460">
+    <row r="460" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G460" s="5"/>
     </row>
-    <row r="461">
+    <row r="461" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G461" s="5"/>
     </row>
-    <row r="462">
+    <row r="462" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G462" s="5"/>
     </row>
-    <row r="463">
+    <row r="463" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G463" s="5"/>
     </row>
-    <row r="464">
+    <row r="464" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G464" s="5"/>
     </row>
-    <row r="465">
+    <row r="465" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G465" s="5"/>
     </row>
-    <row r="466">
+    <row r="466" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G466" s="5"/>
     </row>
-    <row r="467">
+    <row r="467" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G467" s="5"/>
     </row>
-    <row r="468">
+    <row r="468" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G468" s="5"/>
     </row>
-    <row r="469">
+    <row r="469" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G469" s="5"/>
     </row>
-    <row r="470">
+    <row r="470" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G470" s="5"/>
     </row>
-    <row r="471">
+    <row r="471" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G471" s="5"/>
     </row>
-    <row r="472">
+    <row r="472" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G472" s="5"/>
     </row>
-    <row r="473">
+    <row r="473" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G473" s="5"/>
     </row>
-    <row r="474">
+    <row r="474" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G474" s="5"/>
     </row>
-    <row r="475">
+    <row r="475" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G475" s="5"/>
     </row>
-    <row r="476">
+    <row r="476" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G476" s="5"/>
     </row>
-    <row r="477">
+    <row r="477" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G477" s="5"/>
     </row>
-    <row r="478">
+    <row r="478" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G478" s="5"/>
     </row>
-    <row r="479">
+    <row r="479" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G479" s="5"/>
     </row>
-    <row r="480">
+    <row r="480" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G480" s="5"/>
     </row>
-    <row r="481">
+    <row r="481" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G481" s="5"/>
     </row>
-    <row r="482">
+    <row r="482" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G482" s="5"/>
     </row>
-    <row r="483">
+    <row r="483" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G483" s="5"/>
     </row>
-    <row r="484">
+    <row r="484" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G484" s="5"/>
     </row>
-    <row r="485">
+    <row r="485" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G485" s="5"/>
     </row>
-    <row r="486">
+    <row r="486" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G486" s="5"/>
     </row>
-    <row r="487">
+    <row r="487" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G487" s="5"/>
     </row>
-    <row r="488">
+    <row r="488" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G488" s="5"/>
     </row>
-    <row r="489">
+    <row r="489" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G489" s="5"/>
     </row>
-    <row r="490">
+    <row r="490" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G490" s="5"/>
     </row>
-    <row r="491">
+    <row r="491" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G491" s="5"/>
     </row>
-    <row r="492">
+    <row r="492" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G492" s="5"/>
     </row>
-    <row r="493">
+    <row r="493" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G493" s="5"/>
     </row>
-    <row r="494">
+    <row r="494" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G494" s="5"/>
     </row>
-    <row r="495">
+    <row r="495" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G495" s="5"/>
     </row>
-    <row r="496">
+    <row r="496" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G496" s="5"/>
     </row>
-    <row r="497">
+    <row r="497" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G497" s="5"/>
     </row>
-    <row r="498">
+    <row r="498" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G498" s="5"/>
     </row>
-    <row r="499">
+    <row r="499" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G499" s="5"/>
     </row>
-    <row r="500">
+    <row r="500" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G500" s="5"/>
     </row>
-    <row r="501">
+    <row r="501" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G501" s="5"/>
     </row>
-    <row r="502">
+    <row r="502" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G502" s="5"/>
     </row>
-    <row r="503">
+    <row r="503" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G503" s="5"/>
     </row>
-    <row r="504">
+    <row r="504" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G504" s="5"/>
     </row>
-    <row r="505">
+    <row r="505" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G505" s="5"/>
     </row>
-    <row r="506">
+    <row r="506" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G506" s="5"/>
     </row>
-    <row r="507">
+    <row r="507" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G507" s="5"/>
     </row>
-    <row r="508">
+    <row r="508" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G508" s="5"/>
     </row>
-    <row r="509">
+    <row r="509" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G509" s="5"/>
     </row>
-    <row r="510">
+    <row r="510" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G510" s="5"/>
     </row>
-    <row r="511">
+    <row r="511" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G511" s="5"/>
     </row>
-    <row r="512">
+    <row r="512" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G512" s="5"/>
     </row>
-    <row r="513">
+    <row r="513" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G513" s="5"/>
     </row>
-    <row r="514">
+    <row r="514" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G514" s="5"/>
     </row>
-    <row r="515">
+    <row r="515" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G515" s="5"/>
     </row>
-    <row r="516">
+    <row r="516" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G516" s="5"/>
     </row>
-    <row r="517">
+    <row r="517" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G517" s="5"/>
     </row>
-    <row r="518">
+    <row r="518" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G518" s="5"/>
     </row>
-    <row r="519">
+    <row r="519" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G519" s="5"/>
     </row>
-    <row r="520">
+    <row r="520" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G520" s="5"/>
     </row>
-    <row r="521">
+    <row r="521" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G521" s="5"/>
     </row>
-    <row r="522">
+    <row r="522" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G522" s="5"/>
     </row>
-    <row r="523">
+    <row r="523" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G523" s="5"/>
     </row>
-    <row r="524">
+    <row r="524" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G524" s="5"/>
     </row>
-    <row r="525">
+    <row r="525" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G525" s="5"/>
     </row>
-    <row r="526">
+    <row r="526" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G526" s="5"/>
     </row>
-    <row r="527">
+    <row r="527" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G527" s="5"/>
     </row>
-    <row r="528">
+    <row r="528" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G528" s="5"/>
     </row>
-    <row r="529">
+    <row r="529" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G529" s="5"/>
     </row>
-    <row r="530">
+    <row r="530" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G530" s="5"/>
     </row>
-    <row r="531">
+    <row r="531" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G531" s="5"/>
     </row>
-    <row r="532">
+    <row r="532" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G532" s="5"/>
     </row>
-    <row r="533">
+    <row r="533" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G533" s="5"/>
     </row>
-    <row r="534">
+    <row r="534" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G534" s="5"/>
     </row>
-    <row r="535">
+    <row r="535" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G535" s="5"/>
     </row>
-    <row r="536">
+    <row r="536" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G536" s="5"/>
     </row>
-    <row r="537">
+    <row r="537" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G537" s="5"/>
     </row>
-    <row r="538">
+    <row r="538" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G538" s="5"/>
     </row>
-    <row r="539">
+    <row r="539" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G539" s="5"/>
     </row>
-    <row r="540">
+    <row r="540" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G540" s="5"/>
     </row>
-    <row r="541">
+    <row r="541" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G541" s="5"/>
     </row>
-    <row r="542">
+    <row r="542" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G542" s="5"/>
     </row>
-    <row r="543">
+    <row r="543" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G543" s="5"/>
     </row>
-    <row r="544">
+    <row r="544" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G544" s="5"/>
     </row>
-    <row r="545">
+    <row r="545" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G545" s="5"/>
     </row>
-    <row r="546">
+    <row r="546" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G546" s="5"/>
     </row>
-    <row r="547">
+    <row r="547" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G547" s="5"/>
     </row>
-    <row r="548">
+    <row r="548" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G548" s="5"/>
     </row>
-    <row r="549">
+    <row r="549" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G549" s="5"/>
     </row>
-    <row r="550">
+    <row r="550" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G550" s="5"/>
     </row>
-    <row r="551">
+    <row r="551" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G551" s="5"/>
     </row>
-    <row r="552">
+    <row r="552" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G552" s="5"/>
     </row>
-    <row r="553">
+    <row r="553" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G553" s="5"/>
     </row>
-    <row r="554">
+    <row r="554" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G554" s="5"/>
     </row>
-    <row r="555">
+    <row r="555" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G555" s="5"/>
     </row>
-    <row r="556">
+    <row r="556" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G556" s="5"/>
     </row>
-    <row r="557">
+    <row r="557" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G557" s="5"/>
     </row>
-    <row r="558">
+    <row r="558" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G558" s="5"/>
     </row>
-    <row r="559">
+    <row r="559" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G559" s="5"/>
     </row>
-    <row r="560">
+    <row r="560" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G560" s="5"/>
     </row>
-    <row r="561">
+    <row r="561" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G561" s="5"/>
     </row>
-    <row r="562">
+    <row r="562" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G562" s="5"/>
     </row>
-    <row r="563">
+    <row r="563" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G563" s="5"/>
     </row>
-    <row r="564">
+    <row r="564" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G564" s="5"/>
     </row>
-    <row r="565">
+    <row r="565" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G565" s="5"/>
     </row>
-    <row r="566">
+    <row r="566" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G566" s="5"/>
     </row>
-    <row r="567">
+    <row r="567" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G567" s="5"/>
     </row>
-    <row r="568">
+    <row r="568" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G568" s="5"/>
     </row>
-    <row r="569">
+    <row r="569" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G569" s="5"/>
     </row>
-    <row r="570">
+    <row r="570" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G570" s="5"/>
     </row>
-    <row r="571">
+    <row r="571" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G571" s="5"/>
     </row>
-    <row r="572">
+    <row r="572" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G572" s="5"/>
     </row>
-    <row r="573">
+    <row r="573" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G573" s="5"/>
     </row>
-    <row r="574">
+    <row r="574" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G574" s="5"/>
     </row>
-    <row r="575">
+    <row r="575" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G575" s="5"/>
     </row>
-    <row r="576">
+    <row r="576" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G576" s="5"/>
     </row>
-    <row r="577">
+    <row r="577" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G577" s="5"/>
     </row>
-    <row r="578">
+    <row r="578" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G578" s="5"/>
     </row>
-    <row r="579">
+    <row r="579" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G579" s="5"/>
     </row>
-    <row r="580">
+    <row r="580" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G580" s="5"/>
     </row>
-    <row r="581">
+    <row r="581" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G581" s="5"/>
     </row>
-    <row r="582">
+    <row r="582" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G582" s="5"/>
     </row>
-    <row r="583">
+    <row r="583" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G583" s="5"/>
     </row>
-    <row r="584">
+    <row r="584" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G584" s="5"/>
     </row>
-    <row r="585">
+    <row r="585" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G585" s="5"/>
     </row>
-    <row r="586">
+    <row r="586" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G586" s="5"/>
     </row>
-    <row r="587">
+    <row r="587" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G587" s="5"/>
     </row>
-    <row r="588">
+    <row r="588" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G588" s="5"/>
     </row>
-    <row r="589">
+    <row r="589" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G589" s="5"/>
     </row>
-    <row r="590">
+    <row r="590" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G590" s="5"/>
     </row>
-    <row r="591">
+    <row r="591" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G591" s="5"/>
     </row>
-    <row r="592">
+    <row r="592" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G592" s="5"/>
     </row>
-    <row r="593">
+    <row r="593" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G593" s="5"/>
     </row>
-    <row r="594">
+    <row r="594" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G594" s="5"/>
     </row>
-    <row r="595">
+    <row r="595" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G595" s="5"/>
     </row>
-    <row r="596">
+    <row r="596" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G596" s="5"/>
     </row>
-    <row r="597">
+    <row r="597" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G597" s="5"/>
     </row>
-    <row r="598">
+    <row r="598" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G598" s="5"/>
     </row>
-    <row r="599">
+    <row r="599" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G599" s="5"/>
     </row>
-    <row r="600">
+    <row r="600" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G600" s="5"/>
     </row>
-    <row r="601">
+    <row r="601" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G601" s="5"/>
     </row>
-    <row r="602">
+    <row r="602" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G602" s="5"/>
     </row>
-    <row r="603">
+    <row r="603" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G603" s="5"/>
     </row>
-    <row r="604">
+    <row r="604" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G604" s="5"/>
     </row>
-    <row r="605">
+    <row r="605" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G605" s="5"/>
     </row>
-    <row r="606">
+    <row r="606" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G606" s="5"/>
     </row>
-    <row r="607">
+    <row r="607" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G607" s="5"/>
     </row>
-    <row r="608">
+    <row r="608" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G608" s="5"/>
     </row>
-    <row r="609">
+    <row r="609" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G609" s="5"/>
     </row>
-    <row r="610">
+    <row r="610" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G610" s="5"/>
     </row>
-    <row r="611">
+    <row r="611" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G611" s="5"/>
     </row>
-    <row r="612">
+    <row r="612" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G612" s="5"/>
     </row>
-    <row r="613">
+    <row r="613" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G613" s="5"/>
     </row>
-    <row r="614">
+    <row r="614" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G614" s="5"/>
     </row>
-    <row r="615">
+    <row r="615" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G615" s="5"/>
     </row>
-    <row r="616">
+    <row r="616" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G616" s="5"/>
     </row>
-    <row r="617">
+    <row r="617" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G617" s="5"/>
     </row>
-    <row r="618">
+    <row r="618" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G618" s="5"/>
     </row>
-    <row r="619">
+    <row r="619" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G619" s="5"/>
     </row>
-    <row r="620">
+    <row r="620" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G620" s="5"/>
     </row>
-    <row r="621">
+    <row r="621" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G621" s="5"/>
     </row>
-    <row r="622">
+    <row r="622" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G622" s="5"/>
     </row>
-    <row r="623">
+    <row r="623" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G623" s="5"/>
     </row>
-    <row r="624">
+    <row r="624" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G624" s="5"/>
     </row>
-    <row r="625">
+    <row r="625" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G625" s="5"/>
     </row>
-    <row r="626">
+    <row r="626" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G626" s="5"/>
     </row>
-    <row r="627">
+    <row r="627" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G627" s="5"/>
     </row>
-    <row r="628">
+    <row r="628" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G628" s="5"/>
     </row>
-    <row r="629">
+    <row r="629" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G629" s="5"/>
     </row>
-    <row r="630">
+    <row r="630" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G630" s="5"/>
     </row>
-    <row r="631">
+    <row r="631" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G631" s="5"/>
     </row>
-    <row r="632">
+    <row r="632" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G632" s="5"/>
     </row>
-    <row r="633">
+    <row r="633" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G633" s="5"/>
     </row>
-    <row r="634">
+    <row r="634" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G634" s="5"/>
     </row>
-    <row r="635">
+    <row r="635" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G635" s="5"/>
     </row>
-    <row r="636">
+    <row r="636" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G636" s="5"/>
     </row>
-    <row r="637">
+    <row r="637" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G637" s="5"/>
     </row>
-    <row r="638">
+    <row r="638" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G638" s="5"/>
     </row>
-    <row r="639">
+    <row r="639" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G639" s="5"/>
     </row>
-    <row r="640">
+    <row r="640" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G640" s="5"/>
     </row>
-    <row r="641">
+    <row r="641" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G641" s="5"/>
     </row>
-    <row r="642">
+    <row r="642" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G642" s="5"/>
     </row>
-    <row r="643">
+    <row r="643" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G643" s="5"/>
     </row>
-    <row r="644">
+    <row r="644" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G644" s="5"/>
     </row>
-    <row r="645">
+    <row r="645" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G645" s="5"/>
     </row>
-    <row r="646">
+    <row r="646" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G646" s="5"/>
     </row>
-    <row r="647">
+    <row r="647" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G647" s="5"/>
     </row>
-    <row r="648">
+    <row r="648" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G648" s="5"/>
     </row>
-    <row r="649">
+    <row r="649" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G649" s="5"/>
     </row>
-    <row r="650">
+    <row r="650" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G650" s="5"/>
     </row>
-    <row r="651">
+    <row r="651" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G651" s="5"/>
     </row>
-    <row r="652">
+    <row r="652" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G652" s="5"/>
     </row>
-    <row r="653">
+    <row r="653" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G653" s="5"/>
     </row>
-    <row r="654">
+    <row r="654" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G654" s="5"/>
     </row>
-    <row r="655">
+    <row r="655" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G655" s="5"/>
     </row>
-    <row r="656">
+    <row r="656" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G656" s="5"/>
     </row>
-    <row r="657">
+    <row r="657" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G657" s="5"/>
     </row>
-    <row r="658">
+    <row r="658" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G658" s="5"/>
     </row>
-    <row r="659">
+    <row r="659" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G659" s="5"/>
     </row>
-    <row r="660">
+    <row r="660" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G660" s="5"/>
     </row>
-    <row r="661">
+    <row r="661" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G661" s="5"/>
     </row>
-    <row r="662">
+    <row r="662" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G662" s="5"/>
     </row>
-    <row r="663">
+    <row r="663" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G663" s="5"/>
     </row>
-    <row r="664">
+    <row r="664" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G664" s="5"/>
     </row>
-    <row r="665">
+    <row r="665" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G665" s="5"/>
     </row>
-    <row r="666">
+    <row r="666" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G666" s="5"/>
     </row>
-    <row r="667">
+    <row r="667" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G667" s="5"/>
     </row>
-    <row r="668">
+    <row r="668" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G668" s="5"/>
     </row>
-    <row r="669">
+    <row r="669" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G669" s="5"/>
     </row>
-    <row r="670">
+    <row r="670" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G670" s="5"/>
     </row>
-    <row r="671">
+    <row r="671" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G671" s="5"/>
     </row>
-    <row r="672">
+    <row r="672" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G672" s="5"/>
     </row>
-    <row r="673">
+    <row r="673" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G673" s="5"/>
     </row>
-    <row r="674">
+    <row r="674" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G674" s="5"/>
     </row>
-    <row r="675">
+    <row r="675" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G675" s="5"/>
     </row>
-    <row r="676">
+    <row r="676" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G676" s="5"/>
     </row>
-    <row r="677">
+    <row r="677" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G677" s="5"/>
     </row>
-    <row r="678">
+    <row r="678" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G678" s="5"/>
     </row>
-    <row r="679">
+    <row r="679" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G679" s="5"/>
     </row>
-    <row r="680">
+    <row r="680" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G680" s="5"/>
     </row>
-    <row r="681">
+    <row r="681" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G681" s="5"/>
     </row>
-    <row r="682">
+    <row r="682" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G682" s="5"/>
     </row>
-    <row r="683">
+    <row r="683" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G683" s="5"/>
     </row>
-    <row r="684">
+    <row r="684" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G684" s="5"/>
     </row>
-    <row r="685">
+    <row r="685" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G685" s="5"/>
     </row>
-    <row r="686">
+    <row r="686" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G686" s="5"/>
     </row>
-    <row r="687">
+    <row r="687" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G687" s="5"/>
     </row>
-    <row r="688">
+    <row r="688" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G688" s="5"/>
     </row>
-    <row r="689">
+    <row r="689" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G689" s="5"/>
     </row>
-    <row r="690">
+    <row r="690" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G690" s="5"/>
     </row>
-    <row r="691">
+    <row r="691" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G691" s="5"/>
     </row>
-    <row r="692">
+    <row r="692" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G692" s="5"/>
     </row>
-    <row r="693">
+    <row r="693" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G693" s="5"/>
     </row>
-    <row r="694">
+    <row r="694" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G694" s="5"/>
     </row>
-    <row r="695">
+    <row r="695" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G695" s="5"/>
     </row>
-    <row r="696">
+    <row r="696" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G696" s="5"/>
     </row>
-    <row r="697">
+    <row r="697" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G697" s="5"/>
     </row>
-    <row r="698">
+    <row r="698" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G698" s="5"/>
     </row>
-    <row r="699">
+    <row r="699" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G699" s="5"/>
     </row>
-    <row r="700">
+    <row r="700" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G700" s="5"/>
     </row>
-    <row r="701">
+    <row r="701" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G701" s="5"/>
     </row>
-    <row r="702">
+    <row r="702" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G702" s="5"/>
     </row>
-    <row r="703">
+    <row r="703" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G703" s="5"/>
     </row>
-    <row r="704">
+    <row r="704" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G704" s="5"/>
     </row>
-    <row r="705">
+    <row r="705" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G705" s="5"/>
     </row>
-    <row r="706">
+    <row r="706" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G706" s="5"/>
     </row>
-    <row r="707">
+    <row r="707" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G707" s="5"/>
     </row>
-    <row r="708">
+    <row r="708" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G708" s="5"/>
     </row>
-    <row r="709">
+    <row r="709" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G709" s="5"/>
     </row>
-    <row r="710">
+    <row r="710" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G710" s="5"/>
     </row>
-    <row r="711">
+    <row r="711" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G711" s="5"/>
     </row>
-    <row r="712">
+    <row r="712" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G712" s="5"/>
     </row>
-    <row r="713">
+    <row r="713" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G713" s="5"/>
     </row>
-    <row r="714">
+    <row r="714" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G714" s="5"/>
     </row>
-    <row r="715">
+    <row r="715" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G715" s="5"/>
     </row>
-    <row r="716">
+    <row r="716" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G716" s="5"/>
     </row>
-    <row r="717">
+    <row r="717" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G717" s="5"/>
     </row>
-    <row r="718">
+    <row r="718" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G718" s="5"/>
     </row>
-    <row r="719">
+    <row r="719" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G719" s="5"/>
     </row>
-    <row r="720">
+    <row r="720" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G720" s="5"/>
     </row>
-    <row r="721">
+    <row r="721" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G721" s="5"/>
     </row>
-    <row r="722">
+    <row r="722" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G722" s="5"/>
     </row>
-    <row r="723">
+    <row r="723" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G723" s="5"/>
     </row>
-    <row r="724">
+    <row r="724" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G724" s="5"/>
     </row>
-    <row r="725">
+    <row r="725" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G725" s="5"/>
     </row>
-    <row r="726">
+    <row r="726" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G726" s="5"/>
     </row>
-    <row r="727">
+    <row r="727" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G727" s="5"/>
     </row>
-    <row r="728">
+    <row r="728" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G728" s="5"/>
     </row>
-    <row r="729">
+    <row r="729" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G729" s="5"/>
     </row>
-    <row r="730">
+    <row r="730" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G730" s="5"/>
     </row>
-    <row r="731">
+    <row r="731" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G731" s="5"/>
     </row>
-    <row r="732">
+    <row r="732" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G732" s="5"/>
     </row>
-    <row r="733">
+    <row r="733" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G733" s="5"/>
     </row>
-    <row r="734">
+    <row r="734" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G734" s="5"/>
     </row>
-    <row r="735">
+    <row r="735" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G735" s="5"/>
     </row>
-    <row r="736">
+    <row r="736" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G736" s="5"/>
     </row>
-    <row r="737">
+    <row r="737" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G737" s="5"/>
     </row>
-    <row r="738">
+    <row r="738" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G738" s="5"/>
     </row>
-    <row r="739">
+    <row r="739" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G739" s="5"/>
     </row>
-    <row r="740">
+    <row r="740" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G740" s="5"/>
     </row>
-    <row r="741">
+    <row r="741" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G741" s="5"/>
     </row>
-    <row r="742">
+    <row r="742" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G742" s="5"/>
     </row>
-    <row r="743">
+    <row r="743" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G743" s="5"/>
     </row>
-    <row r="744">
+    <row r="744" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G744" s="5"/>
     </row>
-    <row r="745">
+    <row r="745" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G745" s="5"/>
     </row>
-    <row r="746">
+    <row r="746" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G746" s="5"/>
     </row>
-    <row r="747">
+    <row r="747" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G747" s="5"/>
     </row>
-    <row r="748">
+    <row r="748" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G748" s="5"/>
     </row>
-    <row r="749">
+    <row r="749" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G749" s="5"/>
     </row>
-    <row r="750">
+    <row r="750" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G750" s="5"/>
     </row>
-    <row r="751">
+    <row r="751" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G751" s="5"/>
     </row>
-    <row r="752">
+    <row r="752" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G752" s="5"/>
     </row>
-    <row r="753">
+    <row r="753" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G753" s="5"/>
     </row>
-    <row r="754">
+    <row r="754" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G754" s="5"/>
     </row>
-    <row r="755">
+    <row r="755" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G755" s="5"/>
     </row>
-    <row r="756">
+    <row r="756" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G756" s="5"/>
     </row>
-    <row r="757">
+    <row r="757" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G757" s="5"/>
     </row>
-    <row r="758">
+    <row r="758" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G758" s="5"/>
     </row>
-    <row r="759">
+    <row r="759" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G759" s="5"/>
     </row>
-    <row r="760">
+    <row r="760" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G760" s="5"/>
     </row>
-    <row r="761">
+    <row r="761" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G761" s="5"/>
     </row>
-    <row r="762">
+    <row r="762" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G762" s="5"/>
     </row>
-    <row r="763">
+    <row r="763" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G763" s="5"/>
     </row>
-    <row r="764">
+    <row r="764" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G764" s="5"/>
     </row>
-    <row r="765">
+    <row r="765" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G765" s="5"/>
     </row>
-    <row r="766">
+    <row r="766" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G766" s="5"/>
     </row>
-    <row r="767">
+    <row r="767" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G767" s="5"/>
     </row>
-    <row r="768">
+    <row r="768" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G768" s="5"/>
     </row>
-    <row r="769">
+    <row r="769" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G769" s="5"/>
     </row>
-    <row r="770">
+    <row r="770" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G770" s="5"/>
     </row>
-    <row r="771">
+    <row r="771" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G771" s="5"/>
     </row>
-    <row r="772">
+    <row r="772" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G772" s="5"/>
     </row>
-    <row r="773">
+    <row r="773" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G773" s="5"/>
     </row>
-    <row r="774">
+    <row r="774" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G774" s="5"/>
     </row>
-    <row r="775">
+    <row r="775" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G775" s="5"/>
     </row>
-    <row r="776">
+    <row r="776" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G776" s="5"/>
     </row>
-    <row r="777">
+    <row r="777" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G777" s="5"/>
     </row>
-    <row r="778">
+    <row r="778" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G778" s="5"/>
     </row>
-    <row r="779">
+    <row r="779" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G779" s="5"/>
     </row>
-    <row r="780">
+    <row r="780" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G780" s="5"/>
     </row>
-    <row r="781">
+    <row r="781" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G781" s="5"/>
     </row>
-    <row r="782">
+    <row r="782" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G782" s="5"/>
     </row>
-    <row r="783">
+    <row r="783" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G783" s="5"/>
     </row>
-    <row r="784">
+    <row r="784" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G784" s="5"/>
     </row>
-    <row r="785">
+    <row r="785" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G785" s="5"/>
     </row>
-    <row r="786">
+    <row r="786" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G786" s="5"/>
     </row>
-    <row r="787">
+    <row r="787" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G787" s="5"/>
     </row>
-    <row r="788">
+    <row r="788" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G788" s="5"/>
     </row>
-    <row r="789">
+    <row r="789" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G789" s="5"/>
     </row>
-    <row r="790">
+    <row r="790" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G790" s="5"/>
     </row>
-    <row r="791">
+    <row r="791" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G791" s="5"/>
     </row>
-    <row r="792">
+    <row r="792" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G792" s="5"/>
     </row>
-    <row r="793">
+    <row r="793" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G793" s="5"/>
     </row>
-    <row r="794">
+    <row r="794" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G794" s="5"/>
     </row>
-    <row r="795">
+    <row r="795" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G795" s="5"/>
     </row>
-    <row r="796">
+    <row r="796" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G796" s="5"/>
     </row>
-    <row r="797">
+    <row r="797" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G797" s="5"/>
     </row>
-    <row r="798">
+    <row r="798" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G798" s="5"/>
     </row>
-    <row r="799">
+    <row r="799" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G799" s="5"/>
     </row>
-    <row r="800">
+    <row r="800" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G800" s="5"/>
     </row>
-    <row r="801">
+    <row r="801" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G801" s="5"/>
     </row>
-    <row r="802">
+    <row r="802" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G802" s="5"/>
     </row>
-    <row r="803">
+    <row r="803" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G803" s="5"/>
     </row>
-    <row r="804">
+    <row r="804" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G804" s="5"/>
     </row>
-    <row r="805">
+    <row r="805" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G805" s="5"/>
     </row>
-    <row r="806">
+    <row r="806" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G806" s="5"/>
     </row>
-    <row r="807">
+    <row r="807" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G807" s="5"/>
     </row>
-    <row r="808">
+    <row r="808" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G808" s="5"/>
     </row>
-    <row r="809">
+    <row r="809" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G809" s="5"/>
     </row>
-    <row r="810">
+    <row r="810" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G810" s="5"/>
     </row>
-    <row r="811">
+    <row r="811" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G811" s="5"/>
     </row>
-    <row r="812">
+    <row r="812" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G812" s="5"/>
     </row>
-    <row r="813">
+    <row r="813" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G813" s="5"/>
     </row>
-    <row r="814">
+    <row r="814" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G814" s="5"/>
     </row>
-    <row r="815">
+    <row r="815" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G815" s="5"/>
     </row>
-    <row r="816">
+    <row r="816" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G816" s="5"/>
     </row>
-    <row r="817">
+    <row r="817" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G817" s="5"/>
     </row>
-    <row r="818">
+    <row r="818" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G818" s="5"/>
     </row>
-    <row r="819">
+    <row r="819" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G819" s="5"/>
     </row>
-    <row r="820">
+    <row r="820" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G820" s="5"/>
     </row>
-    <row r="821">
+    <row r="821" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G821" s="5"/>
     </row>
-    <row r="822">
+    <row r="822" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G822" s="5"/>
     </row>
-    <row r="823">
+    <row r="823" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G823" s="5"/>
     </row>
-    <row r="824">
+    <row r="824" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G824" s="5"/>
     </row>
-    <row r="825">
+    <row r="825" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G825" s="5"/>
     </row>
-    <row r="826">
+    <row r="826" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G826" s="5"/>
     </row>
-    <row r="827">
+    <row r="827" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G827" s="5"/>
     </row>
-    <row r="828">
+    <row r="828" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G828" s="5"/>
     </row>
-    <row r="829">
+    <row r="829" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G829" s="5"/>
     </row>
-    <row r="830">
+    <row r="830" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G830" s="5"/>
     </row>
-    <row r="831">
+    <row r="831" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G831" s="5"/>
     </row>
-    <row r="832">
+    <row r="832" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G832" s="5"/>
     </row>
-    <row r="833">
+    <row r="833" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G833" s="5"/>
     </row>
-    <row r="834">
+    <row r="834" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G834" s="5"/>
     </row>
-    <row r="835">
+    <row r="835" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G835" s="5"/>
     </row>
-    <row r="836">
+    <row r="836" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G836" s="5"/>
     </row>
-    <row r="837">
+    <row r="837" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G837" s="5"/>
     </row>
-    <row r="838">
+    <row r="838" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G838" s="5"/>
     </row>
-    <row r="839">
+    <row r="839" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G839" s="5"/>
     </row>
-    <row r="840">
+    <row r="840" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G840" s="5"/>
     </row>
-    <row r="841">
+    <row r="841" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G841" s="5"/>
     </row>
-    <row r="842">
+    <row r="842" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G842" s="5"/>
     </row>
-    <row r="843">
+    <row r="843" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G843" s="5"/>
     </row>
-    <row r="844">
+    <row r="844" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G844" s="5"/>
     </row>
-    <row r="845">
+    <row r="845" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G845" s="5"/>
     </row>
-    <row r="846">
+    <row r="846" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G846" s="5"/>
     </row>
-    <row r="847">
+    <row r="847" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G847" s="5"/>
     </row>
-    <row r="848">
+    <row r="848" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G848" s="5"/>
     </row>
-    <row r="849">
+    <row r="849" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G849" s="5"/>
     </row>
-    <row r="850">
+    <row r="850" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G850" s="5"/>
     </row>
-    <row r="851">
+    <row r="851" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G851" s="5"/>
     </row>
-    <row r="852">
+    <row r="852" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G852" s="5"/>
     </row>
-    <row r="853">
+    <row r="853" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G853" s="5"/>
     </row>
-    <row r="854">
+    <row r="854" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G854" s="5"/>
     </row>
-    <row r="855">
+    <row r="855" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G855" s="5"/>
     </row>
-    <row r="856">
+    <row r="856" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G856" s="5"/>
     </row>
-    <row r="857">
+    <row r="857" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G857" s="5"/>
     </row>
-    <row r="858">
+    <row r="858" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G858" s="5"/>
     </row>
-    <row r="859">
+    <row r="859" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G859" s="5"/>
     </row>
-    <row r="860">
+    <row r="860" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G860" s="5"/>
     </row>
-    <row r="861">
+    <row r="861" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G861" s="5"/>
     </row>
-    <row r="862">
+    <row r="862" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G862" s="5"/>
     </row>
-    <row r="863">
+    <row r="863" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G863" s="5"/>
     </row>
-    <row r="864">
+    <row r="864" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G864" s="5"/>
     </row>
-    <row r="865">
+    <row r="865" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G865" s="5"/>
     </row>
-    <row r="866">
+    <row r="866" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G866" s="5"/>
     </row>
-    <row r="867">
+    <row r="867" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G867" s="5"/>
     </row>
-    <row r="868">
+    <row r="868" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G868" s="5"/>
     </row>
-    <row r="869">
+    <row r="869" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G869" s="5"/>
     </row>
-    <row r="870">
+    <row r="870" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G870" s="5"/>
     </row>
-    <row r="871">
+    <row r="871" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G871" s="5"/>
     </row>
-    <row r="872">
+    <row r="872" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G872" s="5"/>
     </row>
-    <row r="873">
+    <row r="873" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G873" s="5"/>
     </row>
-    <row r="874">
+    <row r="874" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G874" s="5"/>
     </row>
-    <row r="875">
+    <row r="875" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G875" s="5"/>
     </row>
-    <row r="876">
+    <row r="876" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G876" s="5"/>
     </row>
-    <row r="877">
+    <row r="877" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G877" s="5"/>
     </row>
-    <row r="878">
+    <row r="878" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G878" s="5"/>
     </row>
-    <row r="879">
+    <row r="879" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G879" s="5"/>
     </row>
-    <row r="880">
+    <row r="880" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G880" s="5"/>
     </row>
-    <row r="881">
+    <row r="881" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G881" s="5"/>
     </row>
-    <row r="882">
+    <row r="882" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G882" s="5"/>
     </row>
-    <row r="883">
+    <row r="883" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G883" s="5"/>
     </row>
-    <row r="884">
+    <row r="884" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G884" s="5"/>
     </row>
-    <row r="885">
+    <row r="885" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G885" s="5"/>
     </row>
-    <row r="886">
+    <row r="886" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G886" s="5"/>
     </row>
-    <row r="887">
+    <row r="887" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G887" s="5"/>
     </row>
-    <row r="888">
+    <row r="888" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G888" s="5"/>
     </row>
-    <row r="889">
+    <row r="889" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G889" s="5"/>
     </row>
-    <row r="890">
+    <row r="890" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G890" s="5"/>
     </row>
-    <row r="891">
+    <row r="891" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G891" s="5"/>
     </row>
-    <row r="892">
+    <row r="892" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G892" s="5"/>
     </row>
-    <row r="893">
+    <row r="893" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G893" s="5"/>
     </row>
-    <row r="894">
+    <row r="894" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G894" s="5"/>
     </row>
-    <row r="895">
+    <row r="895" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G895" s="5"/>
     </row>
-    <row r="896">
+    <row r="896" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G896" s="5"/>
     </row>
-    <row r="897">
+    <row r="897" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G897" s="5"/>
     </row>
-    <row r="898">
+    <row r="898" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G898" s="5"/>
     </row>
-    <row r="899">
+    <row r="899" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G899" s="5"/>
     </row>
-    <row r="900">
+    <row r="900" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G900" s="5"/>
     </row>
-    <row r="901">
+    <row r="901" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G901" s="5"/>
     </row>
-    <row r="902">
+    <row r="902" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G902" s="5"/>
     </row>
-    <row r="903">
+    <row r="903" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G903" s="5"/>
     </row>
-    <row r="904">
+    <row r="904" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G904" s="5"/>
     </row>
-    <row r="905">
+    <row r="905" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G905" s="5"/>
     </row>
-    <row r="906">
+    <row r="906" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G906" s="5"/>
     </row>
-    <row r="907">
+    <row r="907" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G907" s="5"/>
     </row>
-    <row r="908">
+    <row r="908" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G908" s="5"/>
     </row>
-    <row r="909">
+    <row r="909" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G909" s="5"/>
     </row>
-    <row r="910">
+    <row r="910" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G910" s="5"/>
     </row>
-    <row r="911">
+    <row r="911" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G911" s="5"/>
     </row>
-    <row r="912">
+    <row r="912" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G912" s="5"/>
     </row>
-    <row r="913">
+    <row r="913" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G913" s="5"/>
     </row>
-    <row r="914">
+    <row r="914" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G914" s="5"/>
     </row>
-    <row r="915">
+    <row r="915" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G915" s="5"/>
     </row>
-    <row r="916">
+    <row r="916" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G916" s="5"/>
     </row>
-    <row r="917">
+    <row r="917" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G917" s="5"/>
     </row>
-    <row r="918">
+    <row r="918" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G918" s="5"/>
     </row>
-    <row r="919">
+    <row r="919" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G919" s="5"/>
     </row>
-    <row r="920">
+    <row r="920" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G920" s="5"/>
     </row>
-    <row r="921">
+    <row r="921" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G921" s="5"/>
     </row>
-    <row r="922">
+    <row r="922" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G922" s="5"/>
     </row>
-    <row r="923">
+    <row r="923" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G923" s="5"/>
     </row>
-    <row r="924">
+    <row r="924" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G924" s="5"/>
     </row>
-    <row r="925">
+    <row r="925" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G925" s="5"/>
     </row>
-    <row r="926">
+    <row r="926" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G926" s="5"/>
     </row>
-    <row r="927">
+    <row r="927" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G927" s="5"/>
     </row>
-    <row r="928">
+    <row r="928" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G928" s="5"/>
     </row>
-    <row r="929">
+    <row r="929" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G929" s="5"/>
     </row>
-    <row r="930">
+    <row r="930" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G930" s="5"/>
     </row>
-    <row r="931">
+    <row r="931" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G931" s="5"/>
     </row>
-    <row r="932">
+    <row r="932" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G932" s="5"/>
     </row>
-    <row r="933">
+    <row r="933" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G933" s="5"/>
     </row>
-    <row r="934">
+    <row r="934" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G934" s="5"/>
     </row>
-    <row r="935">
+    <row r="935" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G935" s="5"/>
     </row>
-    <row r="936">
+    <row r="936" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G936" s="5"/>
     </row>
-    <row r="937">
+    <row r="937" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G937" s="5"/>
     </row>
-    <row r="938">
+    <row r="938" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G938" s="5"/>
     </row>
-    <row r="939">
+    <row r="939" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G939" s="5"/>
     </row>
-    <row r="940">
+    <row r="940" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G940" s="5"/>
     </row>
-    <row r="941">
+    <row r="941" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G941" s="5"/>
     </row>
-    <row r="942">
+    <row r="942" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G942" s="5"/>
     </row>
-    <row r="943">
+    <row r="943" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G943" s="5"/>
     </row>
-    <row r="944">
+    <row r="944" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G944" s="5"/>
     </row>
-    <row r="945">
+    <row r="945" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G945" s="5"/>
     </row>
-    <row r="946">
+    <row r="946" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G946" s="5"/>
     </row>
-    <row r="947">
+    <row r="947" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G947" s="5"/>
     </row>
-    <row r="948">
+    <row r="948" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G948" s="5"/>
     </row>
-    <row r="949">
+    <row r="949" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G949" s="5"/>
     </row>
-    <row r="950">
+    <row r="950" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G950" s="5"/>
     </row>
-    <row r="951">
+    <row r="951" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G951" s="5"/>
     </row>
-    <row r="952">
+    <row r="952" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G952" s="5"/>
     </row>
-    <row r="953">
+    <row r="953" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G953" s="5"/>
     </row>
-    <row r="954">
+    <row r="954" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G954" s="5"/>
     </row>
-    <row r="955">
+    <row r="955" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G955" s="5"/>
     </row>
-    <row r="956">
+    <row r="956" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G956" s="5"/>
     </row>
-    <row r="957">
+    <row r="957" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G957" s="5"/>
     </row>
-    <row r="958">
+    <row r="958" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G958" s="5"/>
     </row>
-    <row r="959">
+    <row r="959" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G959" s="5"/>
     </row>
-    <row r="960">
+    <row r="960" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G960" s="5"/>
     </row>
-    <row r="961">
+    <row r="961" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G961" s="5"/>
     </row>
-    <row r="962">
+    <row r="962" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G962" s="5"/>
     </row>
-    <row r="963">
+    <row r="963" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G963" s="5"/>
     </row>
-    <row r="964">
+    <row r="964" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G964" s="5"/>
     </row>
-    <row r="965">
+    <row r="965" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G965" s="5"/>
     </row>
-    <row r="966">
+    <row r="966" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G966" s="5"/>
     </row>
-    <row r="967">
+    <row r="967" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G967" s="5"/>
     </row>
-    <row r="968">
+    <row r="968" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G968" s="5"/>
     </row>
-    <row r="969">
+    <row r="969" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G969" s="5"/>
     </row>
-    <row r="970">
+    <row r="970" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G970" s="5"/>
     </row>
-    <row r="971">
+    <row r="971" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G971" s="5"/>
     </row>
-    <row r="972">
+    <row r="972" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G972" s="5"/>
     </row>
-    <row r="973">
+    <row r="973" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G973" s="5"/>
     </row>
-    <row r="974">
+    <row r="974" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G974" s="5"/>
     </row>
-    <row r="975">
+    <row r="975" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G975" s="5"/>
     </row>
-    <row r="976">
+    <row r="976" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G976" s="5"/>
     </row>
-    <row r="977">
+    <row r="977" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G977" s="5"/>
     </row>
-    <row r="978">
+    <row r="978" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G978" s="5"/>
     </row>
-    <row r="979">
+    <row r="979" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G979" s="5"/>
     </row>
-    <row r="980">
+    <row r="980" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G980" s="5"/>
     </row>
-    <row r="981">
+    <row r="981" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G981" s="5"/>
     </row>
-    <row r="982">
+    <row r="982" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G982" s="5"/>
     </row>
-    <row r="983">
+    <row r="983" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G983" s="5"/>
     </row>
-    <row r="984">
+    <row r="984" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G984" s="5"/>
     </row>
-    <row r="985">
+    <row r="985" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G985" s="5"/>
     </row>
-    <row r="986">
+    <row r="986" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G986" s="5"/>
     </row>
-    <row r="987">
+    <row r="987" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G987" s="5"/>
     </row>
-    <row r="988">
+    <row r="988" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G988" s="5"/>
     </row>
-    <row r="989">
+    <row r="989" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G989" s="5"/>
     </row>
-    <row r="990">
+    <row r="990" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G990" s="5"/>
     </row>
-    <row r="991">
+    <row r="991" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G991" s="5"/>
     </row>
-    <row r="992">
+    <row r="992" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G992" s="5"/>
     </row>
-    <row r="993">
+    <row r="993" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G993" s="5"/>
     </row>
-    <row r="994">
+    <row r="994" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G994" s="5"/>
     </row>
-    <row r="995">
+    <row r="995" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G995" s="5"/>
     </row>
-    <row r="996">
+    <row r="996" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G996" s="5"/>
     </row>
-    <row r="997">
+    <row r="997" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G997" s="5"/>
     </row>
-    <row r="998">
+    <row r="998" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G998" s="5"/>
     </row>
-    <row r="999">
+    <row r="999" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G999" s="5"/>
     </row>
-    <row r="1000">
+    <row r="1000" spans="7:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G1000" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>